<commit_message>
adding "general" for Therapist
</commit_message>
<xml_diff>
--- a/Data/acount and passwords.xlsx
+++ b/Data/acount and passwords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Oz\fiveer\Dani_Velinchick\KrohnApp\python_codes\COBIMINDEX\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{128001CE-5346-460C-A0B8-1D08BAD7CDE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39AAD454-B733-4AEA-8166-854BFAA87E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="379">
   <si>
     <t>acount</t>
   </si>
@@ -572,6 +572,9 @@
   </si>
   <si>
     <t>מילכה חנוקוגלו</t>
+  </si>
+  <si>
+    <t>Zohar Peled-Zinger</t>
   </si>
   <si>
     <t>2023-08-21</t>
@@ -1577,7 +1580,7 @@
   <dimension ref="A1:M301"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3353,25 +3356,25 @@
         <v>181</v>
       </c>
       <c r="E152" t="s">
-        <v>17</v>
+        <v>182</v>
       </c>
       <c r="F152" t="s">
         <v>17</v>
       </c>
       <c r="G152" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H152" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I152" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="J152" t="s">
         <v>21</v>
       </c>
       <c r="K152" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="L152" t="s">
         <v>23</v>
@@ -3382,13 +3385,13 @@
         <v>590307</v>
       </c>
       <c r="B153" s="5" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C153" s="5" t="s">
         <v>180</v>
       </c>
       <c r="D153" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E153" t="s">
         <v>17</v>
@@ -3397,19 +3400,19 @@
         <v>17</v>
       </c>
       <c r="G153" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H153" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I153" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="J153" t="s">
         <v>21</v>
       </c>
       <c r="K153" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="154" spans="1:12" x14ac:dyDescent="0.3">
@@ -3417,7 +3420,7 @@
         <v>847633</v>
       </c>
       <c r="B154" s="5" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C154" s="5" t="s">
         <v>180</v>
@@ -3428,34 +3431,34 @@
         <v>538067</v>
       </c>
       <c r="B155" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C155" s="5" t="s">
         <v>180</v>
       </c>
       <c r="D155" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E155" t="s">
-        <v>17</v>
+        <v>182</v>
       </c>
       <c r="F155" t="s">
         <v>17</v>
       </c>
       <c r="G155" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H155" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I155" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="J155" t="s">
         <v>21</v>
       </c>
       <c r="K155" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="156" spans="1:12" x14ac:dyDescent="0.3">
@@ -3463,13 +3466,13 @@
         <v>889142</v>
       </c>
       <c r="B156" s="5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C156" s="5" t="s">
         <v>180</v>
       </c>
       <c r="D156" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E156" t="s">
         <v>17</v>
@@ -3478,19 +3481,19 @@
         <v>17</v>
       </c>
       <c r="G156" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H156" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I156" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="J156" t="s">
         <v>21</v>
       </c>
       <c r="K156" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="157" spans="1:12" x14ac:dyDescent="0.3">
@@ -3498,7 +3501,7 @@
         <v>988429</v>
       </c>
       <c r="B157" s="5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C157" s="5" t="s">
         <v>180</v>
@@ -3509,7 +3512,7 @@
         <v>159320</v>
       </c>
       <c r="B158" s="5" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C158" s="5" t="s">
         <v>180</v>
@@ -3520,13 +3523,13 @@
         <v>985070</v>
       </c>
       <c r="B159" s="5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C159" s="5" t="s">
         <v>180</v>
       </c>
       <c r="D159" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E159" t="s">
         <v>17</v>
@@ -3535,19 +3538,19 @@
         <v>17</v>
       </c>
       <c r="G159" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H159" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I159" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="J159" t="s">
         <v>21</v>
       </c>
       <c r="K159" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="160" spans="1:12" x14ac:dyDescent="0.3">
@@ -3555,7 +3558,7 @@
         <v>872696</v>
       </c>
       <c r="B160" s="5" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C160" s="5" t="s">
         <v>180</v>
@@ -3566,7 +3569,7 @@
         <v>645107</v>
       </c>
       <c r="B161" s="5" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C161" s="5" t="s">
         <v>180</v>
@@ -3577,13 +3580,13 @@
         <v>213190</v>
       </c>
       <c r="B162" s="5" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C162" s="5" t="s">
         <v>180</v>
       </c>
       <c r="D162" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E162" t="s">
         <v>17</v>
@@ -3592,19 +3595,19 @@
         <v>17</v>
       </c>
       <c r="G162" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="H162" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I162" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="J162" t="s">
         <v>21</v>
       </c>
       <c r="K162" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="163" spans="1:11" x14ac:dyDescent="0.3">
@@ -3612,13 +3615,13 @@
         <v>170406</v>
       </c>
       <c r="B163" s="5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C163" s="5" t="s">
         <v>180</v>
       </c>
       <c r="D163" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E163" t="s">
         <v>17</v>
@@ -3627,19 +3630,19 @@
         <v>17</v>
       </c>
       <c r="G163" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H163" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I163" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="J163" t="s">
         <v>21</v>
       </c>
       <c r="K163" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="164" spans="1:11" x14ac:dyDescent="0.3">
@@ -3647,13 +3650,13 @@
         <v>588655</v>
       </c>
       <c r="B164" s="5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C164" s="5" t="s">
         <v>180</v>
       </c>
       <c r="D164" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E164" t="s">
         <v>17</v>
@@ -3662,19 +3665,19 @@
         <v>17</v>
       </c>
       <c r="G164" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="H164" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="I164" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="J164" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="K164" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="165" spans="1:11" x14ac:dyDescent="0.3">
@@ -3682,7 +3685,7 @@
         <v>441310</v>
       </c>
       <c r="B165" s="5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C165" s="5" t="s">
         <v>180</v>
@@ -3693,7 +3696,7 @@
         <v>312435</v>
       </c>
       <c r="B166" s="5" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C166" s="5" t="s">
         <v>180</v>
@@ -3704,7 +3707,7 @@
         <v>505418</v>
       </c>
       <c r="B167" s="5" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C167" s="5" t="s">
         <v>180</v>
@@ -3715,7 +3718,7 @@
         <v>376454</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C168" s="2" t="s">
         <v>180</v>
@@ -3726,7 +3729,7 @@
         <v>123773</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C169" s="2" t="s">
         <v>180</v>
@@ -3737,7 +3740,7 @@
         <v>670053</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C170" s="2" t="s">
         <v>180</v>
@@ -3748,7 +3751,7 @@
         <v>836877</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C171" s="2" t="s">
         <v>180</v>
@@ -3759,7 +3762,7 @@
         <v>416703</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C172" s="2" t="s">
         <v>180</v>
@@ -3770,7 +3773,7 @@
         <v>901595</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C173" s="2" t="s">
         <v>180</v>
@@ -3781,7 +3784,7 @@
         <v>941906</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C174" s="2" t="s">
         <v>180</v>
@@ -3792,7 +3795,7 @@
         <v>627642</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C175" s="2" t="s">
         <v>180</v>
@@ -3803,7 +3806,7 @@
         <v>899270</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C176" s="2" t="s">
         <v>180</v>
@@ -3814,7 +3817,7 @@
         <v>590058</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C177" s="2" t="s">
         <v>180</v>
@@ -3825,7 +3828,7 @@
         <v>371205</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C178" s="2" t="s">
         <v>180</v>
@@ -3836,7 +3839,7 @@
         <v>230657</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C179" s="2" t="s">
         <v>180</v>
@@ -3847,7 +3850,7 @@
         <v>920598</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C180" s="2" t="s">
         <v>180</v>
@@ -3858,7 +3861,7 @@
         <v>248805</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C181" s="2" t="s">
         <v>180</v>
@@ -3869,7 +3872,7 @@
         <v>795262</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C182" s="2" t="s">
         <v>180</v>
@@ -3880,7 +3883,7 @@
         <v>798645</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C183" s="2" t="s">
         <v>180</v>
@@ -3891,7 +3894,7 @@
         <v>525832</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C184" s="2" t="s">
         <v>180</v>
@@ -3902,7 +3905,7 @@
         <v>792144</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C185" s="2" t="s">
         <v>180</v>
@@ -3913,7 +3916,7 @@
         <v>551946</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C186" s="2" t="s">
         <v>180</v>
@@ -3924,7 +3927,7 @@
         <v>499921</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C187" s="2" t="s">
         <v>180</v>
@@ -3935,7 +3938,7 @@
         <v>131181</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C188" s="2" t="s">
         <v>180</v>
@@ -3946,7 +3949,7 @@
         <v>109050</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C189" s="2" t="s">
         <v>180</v>
@@ -3957,7 +3960,7 @@
         <v>814695</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C190" s="2" t="s">
         <v>180</v>
@@ -3968,7 +3971,7 @@
         <v>617288</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C191" s="2" t="s">
         <v>180</v>
@@ -3979,7 +3982,7 @@
         <v>362341</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C192" s="2" t="s">
         <v>180</v>
@@ -3990,7 +3993,7 @@
         <v>168037</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C193" s="2" t="s">
         <v>180</v>
@@ -4001,7 +4004,7 @@
         <v>498906</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C194" s="2" t="s">
         <v>180</v>
@@ -4012,7 +4015,7 @@
         <v>377337</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C195" s="2" t="s">
         <v>180</v>
@@ -4023,7 +4026,7 @@
         <v>153481</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C196" s="2" t="s">
         <v>180</v>
@@ -4034,7 +4037,7 @@
         <v>777608</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C197" s="2" t="s">
         <v>180</v>
@@ -4045,7 +4048,7 @@
         <v>138321</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C198" s="2" t="s">
         <v>180</v>
@@ -4056,7 +4059,7 @@
         <v>940840</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C199" s="2" t="s">
         <v>180</v>
@@ -4067,7 +4070,7 @@
         <v>477622</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C200" s="2" t="s">
         <v>180</v>
@@ -4078,7 +4081,7 @@
         <v>788436</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C201" s="2" t="s">
         <v>180</v>
@@ -4089,7 +4092,7 @@
         <v>124210</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C202" s="2" t="s">
         <v>180</v>
@@ -4100,7 +4103,7 @@
         <v>953959</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C203" s="2" t="s">
         <v>180</v>
@@ -4111,7 +4114,7 @@
         <v>837763</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C204" s="2" t="s">
         <v>180</v>
@@ -4122,7 +4125,7 @@
         <v>955318</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C205" s="2" t="s">
         <v>180</v>
@@ -4133,7 +4136,7 @@
         <v>725305</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C206" s="2" t="s">
         <v>180</v>
@@ -4144,7 +4147,7 @@
         <v>441140</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C207" s="2" t="s">
         <v>180</v>
@@ -4155,7 +4158,7 @@
         <v>140987</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C208" s="2" t="s">
         <v>180</v>
@@ -4166,7 +4169,7 @@
         <v>524829</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C209" s="2" t="s">
         <v>180</v>
@@ -4177,7 +4180,7 @@
         <v>270875</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C210" s="2" t="s">
         <v>180</v>
@@ -4188,7 +4191,7 @@
         <v>295528</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C211" s="2" t="s">
         <v>180</v>
@@ -4199,7 +4202,7 @@
         <v>633362</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C212" s="2" t="s">
         <v>180</v>
@@ -4210,7 +4213,7 @@
         <v>401332</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C213" s="2" t="s">
         <v>180</v>
@@ -4221,7 +4224,7 @@
         <v>867537</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C214" s="2" t="s">
         <v>180</v>
@@ -4232,7 +4235,7 @@
         <v>670080</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C215" s="2" t="s">
         <v>180</v>
@@ -4243,7 +4246,7 @@
         <v>109607</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C216" s="2" t="s">
         <v>180</v>
@@ -4254,7 +4257,7 @@
         <v>253467</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C217" s="2" t="s">
         <v>180</v>
@@ -4265,7 +4268,7 @@
         <v>760025</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C218" s="2" t="s">
         <v>180</v>
@@ -4276,7 +4279,7 @@
         <v>219224</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C219" s="2" t="s">
         <v>180</v>
@@ -4287,7 +4290,7 @@
         <v>236594</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C220" s="2" t="s">
         <v>180</v>
@@ -4298,7 +4301,7 @@
         <v>142340</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C221" s="2" t="s">
         <v>180</v>
@@ -4309,7 +4312,7 @@
         <v>416983</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C222" s="2" t="s">
         <v>180</v>
@@ -4320,7 +4323,7 @@
         <v>162554</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C223" s="2" t="s">
         <v>180</v>
@@ -4331,7 +4334,7 @@
         <v>805552</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C224" s="2" t="s">
         <v>180</v>
@@ -4342,7 +4345,7 @@
         <v>430470</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C225" s="2" t="s">
         <v>180</v>
@@ -4353,7 +4356,7 @@
         <v>682715</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C226" s="2" t="s">
         <v>180</v>
@@ -4364,7 +4367,7 @@
         <v>125422</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C227" s="2" t="s">
         <v>180</v>
@@ -4375,7 +4378,7 @@
         <v>396572</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C228" s="2" t="s">
         <v>180</v>
@@ -4386,7 +4389,7 @@
         <v>837658</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C229" s="2" t="s">
         <v>180</v>
@@ -4397,7 +4400,7 @@
         <v>258437</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C230" s="2" t="s">
         <v>180</v>
@@ -4408,7 +4411,7 @@
         <v>890385</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C231" s="2" t="s">
         <v>180</v>
@@ -4419,7 +4422,7 @@
         <v>664614</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C232" s="2" t="s">
         <v>180</v>
@@ -4430,7 +4433,7 @@
         <v>938321</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C233" s="2" t="s">
         <v>180</v>
@@ -4441,7 +4444,7 @@
         <v>600996</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C234" s="2" t="s">
         <v>180</v>
@@ -4452,7 +4455,7 @@
         <v>480445</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C235" s="2" t="s">
         <v>180</v>
@@ -4463,7 +4466,7 @@
         <v>768723</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C236" s="2" t="s">
         <v>180</v>
@@ -4474,7 +4477,7 @@
         <v>246117</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C237" s="2" t="s">
         <v>180</v>
@@ -4485,7 +4488,7 @@
         <v>125548</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C238" s="2" t="s">
         <v>180</v>
@@ -4496,7 +4499,7 @@
         <v>116030</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C239" s="2" t="s">
         <v>180</v>
@@ -4507,7 +4510,7 @@
         <v>532833</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C240" s="2" t="s">
         <v>180</v>
@@ -4518,7 +4521,7 @@
         <v>258194</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C241" s="2" t="s">
         <v>180</v>
@@ -4529,7 +4532,7 @@
         <v>790649</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C242" s="2" t="s">
         <v>180</v>
@@ -4540,7 +4543,7 @@
         <v>408393</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C243" s="2" t="s">
         <v>180</v>
@@ -4551,7 +4554,7 @@
         <v>130690</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C244" s="2" t="s">
         <v>180</v>
@@ -4562,7 +4565,7 @@
         <v>722019</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C245" s="2" t="s">
         <v>180</v>
@@ -4573,7 +4576,7 @@
         <v>161316</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C246" s="2" t="s">
         <v>180</v>
@@ -4584,7 +4587,7 @@
         <v>130692</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C247" s="2" t="s">
         <v>180</v>
@@ -4595,7 +4598,7 @@
         <v>259516</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C248" s="2" t="s">
         <v>180</v>
@@ -4606,7 +4609,7 @@
         <v>711278</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C249" s="2" t="s">
         <v>180</v>
@@ -4617,7 +4620,7 @@
         <v>604010</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C250" s="2" t="s">
         <v>180</v>
@@ -4628,7 +4631,7 @@
         <v>265571</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C251" s="2" t="s">
         <v>180</v>
@@ -4639,7 +4642,7 @@
         <v>435185</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C252" s="2" t="s">
         <v>180</v>
@@ -4650,7 +4653,7 @@
         <v>298834</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C253" s="2" t="s">
         <v>180</v>
@@ -4661,7 +4664,7 @@
         <v>704753</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C254" s="2" t="s">
         <v>180</v>
@@ -4672,7 +4675,7 @@
         <v>282119</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C255" s="2" t="s">
         <v>180</v>
@@ -4683,7 +4686,7 @@
         <v>961003</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C256" s="2" t="s">
         <v>180</v>
@@ -4694,7 +4697,7 @@
         <v>840316</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C257" s="2" t="s">
         <v>180</v>
@@ -4705,7 +4708,7 @@
         <v>222365</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C258" s="2" t="s">
         <v>180</v>
@@ -4716,7 +4719,7 @@
         <v>539448</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C259" s="2" t="s">
         <v>180</v>
@@ -4727,7 +4730,7 @@
         <v>168232</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C260" s="2" t="s">
         <v>180</v>
@@ -4738,7 +4741,7 @@
         <v>521488</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C261" s="2" t="s">
         <v>180</v>
@@ -4749,7 +4752,7 @@
         <v>367321</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C262" s="2" t="s">
         <v>180</v>
@@ -4760,7 +4763,7 @@
         <v>448880</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C263" s="2" t="s">
         <v>180</v>
@@ -4771,7 +4774,7 @@
         <v>957707</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C264" s="2" t="s">
         <v>180</v>
@@ -4782,7 +4785,7 @@
         <v>545688</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C265" s="2" t="s">
         <v>180</v>
@@ -4793,7 +4796,7 @@
         <v>418967</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C266" s="2" t="s">
         <v>180</v>
@@ -4804,7 +4807,7 @@
         <v>941428</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C267" s="2" t="s">
         <v>180</v>
@@ -4815,7 +4818,7 @@
         <v>347267</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C268" s="2" t="s">
         <v>180</v>
@@ -4826,7 +4829,7 @@
         <v>104372</v>
       </c>
       <c r="B269" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C269" s="2" t="s">
         <v>180</v>
@@ -4837,7 +4840,7 @@
         <v>745171</v>
       </c>
       <c r="B270" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C270" s="2" t="s">
         <v>180</v>
@@ -4848,7 +4851,7 @@
         <v>942780</v>
       </c>
       <c r="B271" s="2" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C271" s="2" t="s">
         <v>180</v>
@@ -4859,7 +4862,7 @@
         <v>925707</v>
       </c>
       <c r="B272" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C272" s="2" t="s">
         <v>180</v>
@@ -4870,7 +4873,7 @@
         <v>735195</v>
       </c>
       <c r="B273" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C273" s="2" t="s">
         <v>180</v>
@@ -4881,7 +4884,7 @@
         <v>882321</v>
       </c>
       <c r="B274" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C274" s="2" t="s">
         <v>180</v>
@@ -4892,7 +4895,7 @@
         <v>907335</v>
       </c>
       <c r="B275" s="2" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C275" s="2" t="s">
         <v>180</v>
@@ -4903,7 +4906,7 @@
         <v>291069</v>
       </c>
       <c r="B276" s="2" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C276" s="2" t="s">
         <v>180</v>
@@ -4914,16 +4917,16 @@
         <v>789271</v>
       </c>
       <c r="B277" s="2" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C277" s="2" t="s">
         <v>180</v>
       </c>
       <c r="D277" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="E277" s="6" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="278" spans="1:12" x14ac:dyDescent="0.3">
@@ -4931,13 +4934,13 @@
         <v>533772</v>
       </c>
       <c r="B278" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C278" s="2" t="s">
         <v>180</v>
       </c>
       <c r="D278" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="E278" s="6" t="s">
         <v>17</v>
@@ -4946,19 +4949,19 @@
         <v>17</v>
       </c>
       <c r="G278" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="H278" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="I278" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="J278" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="K278" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="279" spans="1:12" x14ac:dyDescent="0.3">
@@ -4966,13 +4969,13 @@
         <v>979471</v>
       </c>
       <c r="B279" s="2" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C279" s="2" t="s">
         <v>180</v>
       </c>
       <c r="D279" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="E279" s="6" t="s">
         <v>17</v>
@@ -4981,19 +4984,19 @@
         <v>17</v>
       </c>
       <c r="G279" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H279" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I279" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="J279" t="s">
         <v>21</v>
       </c>
       <c r="K279" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="L279" t="s">
         <v>23</v>
@@ -5004,13 +5007,13 @@
         <v>433534</v>
       </c>
       <c r="B280" s="2" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C280" s="2" t="s">
         <v>180</v>
       </c>
       <c r="D280" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="E280" s="6" t="s">
         <v>17</v>
@@ -5019,19 +5022,19 @@
         <v>17</v>
       </c>
       <c r="G280" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H280" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I280" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="J280" t="s">
         <v>21</v>
       </c>
       <c r="K280" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="281" spans="1:12" x14ac:dyDescent="0.3">
@@ -5039,13 +5042,13 @@
         <v>185957</v>
       </c>
       <c r="B281" s="2" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C281" s="2" t="s">
         <v>180</v>
       </c>
       <c r="D281" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E281" s="6" t="s">
         <v>17</v>
@@ -5054,19 +5057,19 @@
         <v>17</v>
       </c>
       <c r="G281" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H281" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I281" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="J281" t="s">
         <v>21</v>
       </c>
       <c r="K281" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="282" spans="1:12" x14ac:dyDescent="0.3">
@@ -5074,13 +5077,13 @@
         <v>997539</v>
       </c>
       <c r="B282" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C282" s="2" t="s">
         <v>180</v>
       </c>
       <c r="D282" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="E282" s="6" t="s">
         <v>17</v>
@@ -5089,19 +5092,19 @@
         <v>17</v>
       </c>
       <c r="G282" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H282" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I282" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="J282" t="s">
         <v>21</v>
       </c>
       <c r="K282" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="283" spans="1:12" x14ac:dyDescent="0.3">
@@ -5109,13 +5112,13 @@
         <v>581651</v>
       </c>
       <c r="B283" s="2" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C283" s="2" t="s">
         <v>180</v>
       </c>
       <c r="D283" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="E283" s="6" t="s">
         <v>17</v>
@@ -5124,19 +5127,19 @@
         <v>17</v>
       </c>
       <c r="G283" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H283" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I283" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="J283" t="s">
         <v>21</v>
       </c>
       <c r="K283" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="284" spans="1:12" x14ac:dyDescent="0.3">
@@ -5144,13 +5147,13 @@
         <v>493614</v>
       </c>
       <c r="B284" s="2" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C284" s="2" t="s">
         <v>180</v>
       </c>
       <c r="D284" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="E284" s="6" t="s">
         <v>17</v>
@@ -5159,19 +5162,19 @@
         <v>17</v>
       </c>
       <c r="G284" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H284" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I284" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="J284" t="s">
         <v>21</v>
       </c>
       <c r="K284" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="285" spans="1:12" x14ac:dyDescent="0.3">
@@ -5179,13 +5182,13 @@
         <v>869576</v>
       </c>
       <c r="B285" s="2" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C285" s="2" t="s">
         <v>180</v>
       </c>
       <c r="D285" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="E285" s="6" t="s">
         <v>17</v>
@@ -5194,19 +5197,19 @@
         <v>17</v>
       </c>
       <c r="G285" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H285" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I285" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="J285" t="s">
         <v>21</v>
       </c>
       <c r="K285" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="286" spans="1:12" x14ac:dyDescent="0.3">
@@ -5214,13 +5217,13 @@
         <v>166937</v>
       </c>
       <c r="B286" s="2" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C286" s="2" t="s">
         <v>180</v>
       </c>
       <c r="D286" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E286" s="6" t="s">
         <v>17</v>
@@ -5229,22 +5232,22 @@
         <v>17</v>
       </c>
       <c r="G286" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H286" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I286" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="J286" t="s">
         <v>21</v>
       </c>
       <c r="K286" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="L286" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="287" spans="1:12" x14ac:dyDescent="0.3">
@@ -5252,16 +5255,16 @@
         <v>869123</v>
       </c>
       <c r="B287" s="5" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C287" s="5" t="s">
         <v>180</v>
       </c>
       <c r="D287" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="E287" s="6" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="288" spans="1:12" x14ac:dyDescent="0.3">
@@ -5269,16 +5272,16 @@
         <v>300076</v>
       </c>
       <c r="B288" s="5" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C288" s="5" t="s">
         <v>180</v>
       </c>
       <c r="D288" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="E288" s="6" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="289" spans="1:12" x14ac:dyDescent="0.3">
@@ -5286,29 +5289,29 @@
         <v>321843</v>
       </c>
       <c r="B289" s="5" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C289" s="5" t="s">
         <v>180</v>
       </c>
       <c r="D289" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="E289" s="6"/>
       <c r="G289" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H289" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I289" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="J289" t="s">
         <v>21</v>
       </c>
       <c r="K289" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="290" spans="1:12" x14ac:dyDescent="0.3">
@@ -5316,34 +5319,34 @@
         <v>650674</v>
       </c>
       <c r="B290" s="5" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C290" s="5" t="s">
         <v>180</v>
       </c>
       <c r="D290" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="E290" s="6" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="G290" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H290" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I290" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="J290" t="s">
         <v>21</v>
       </c>
       <c r="K290" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="L290" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="291" spans="1:12" x14ac:dyDescent="0.3">
@@ -5351,16 +5354,16 @@
         <v>289205</v>
       </c>
       <c r="B291" s="5" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C291" s="5" t="s">
         <v>180</v>
       </c>
       <c r="D291" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="E291" s="6" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="292" spans="1:12" x14ac:dyDescent="0.3">
@@ -5368,34 +5371,34 @@
         <v>141787</v>
       </c>
       <c r="B292" s="5" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C292" s="5" t="s">
         <v>180</v>
       </c>
       <c r="D292" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="E292" s="6" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="G292" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H292" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I292" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="J292" t="s">
         <v>21</v>
       </c>
       <c r="K292" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="L292" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="293" spans="1:12" x14ac:dyDescent="0.3">
@@ -5403,13 +5406,13 @@
         <v>287679</v>
       </c>
       <c r="B293" s="5" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C293" s="5" t="s">
         <v>180</v>
       </c>
       <c r="D293" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="E293" s="6" t="s">
         <v>17</v>
@@ -5418,19 +5421,19 @@
         <v>17</v>
       </c>
       <c r="G293" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H293" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I293" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="J293" t="s">
         <v>21</v>
       </c>
       <c r="K293" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="294" spans="1:12" x14ac:dyDescent="0.3">
@@ -5438,34 +5441,34 @@
         <v>647487</v>
       </c>
       <c r="B294" s="5" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C294" s="5" t="s">
         <v>180</v>
       </c>
       <c r="D294" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="E294" s="6" t="s">
         <v>17</v>
       </c>
       <c r="F294" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="G294" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H294" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I294" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="J294" t="s">
         <v>21</v>
       </c>
       <c r="K294" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="L294" t="s">
         <v>23</v>
@@ -5476,13 +5479,13 @@
         <v>451487</v>
       </c>
       <c r="B295" s="5" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C295" s="5" t="s">
         <v>180</v>
       </c>
       <c r="D295" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="E295" s="6" t="s">
         <v>17</v>
@@ -5491,22 +5494,22 @@
         <v>17</v>
       </c>
       <c r="G295" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H295" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I295" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="J295" t="s">
         <v>21</v>
       </c>
       <c r="K295" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="L295" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="296" spans="1:12" x14ac:dyDescent="0.3">
@@ -5514,13 +5517,13 @@
         <v>861671</v>
       </c>
       <c r="B296" s="5" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C296" s="5" t="s">
         <v>180</v>
       </c>
       <c r="D296" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="E296" s="6" t="s">
         <v>17</v>
@@ -5529,19 +5532,19 @@
         <v>17</v>
       </c>
       <c r="G296" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H296" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I296" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="J296" t="s">
         <v>21</v>
       </c>
       <c r="K296" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="297" spans="1:12" x14ac:dyDescent="0.3">
@@ -5549,13 +5552,13 @@
         <v>316094</v>
       </c>
       <c r="B297" s="5" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C297" s="5" t="s">
         <v>180</v>
       </c>
       <c r="D297" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="E297" s="6" t="s">
         <v>17</v>
@@ -5564,19 +5567,19 @@
         <v>17</v>
       </c>
       <c r="G297" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H297" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I297" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="J297" t="s">
         <v>21</v>
       </c>
       <c r="K297" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="298" spans="1:12" x14ac:dyDescent="0.3">
@@ -5584,13 +5587,13 @@
         <v>924424</v>
       </c>
       <c r="B298" s="5" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C298" s="5" t="s">
         <v>180</v>
       </c>
       <c r="D298" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="E298" s="6" t="s">
         <v>17</v>
@@ -5599,19 +5602,19 @@
         <v>17</v>
       </c>
       <c r="G298" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H298" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I298" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="J298" t="s">
         <v>21</v>
       </c>
       <c r="K298" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="299" spans="1:12" x14ac:dyDescent="0.3">
@@ -5619,13 +5622,13 @@
         <v>918170</v>
       </c>
       <c r="B299" s="5" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C299" s="5" t="s">
         <v>180</v>
       </c>
       <c r="D299" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="E299" s="6" t="s">
         <v>17</v>
@@ -5634,19 +5637,19 @@
         <v>17</v>
       </c>
       <c r="G299" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H299" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I299" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="J299" t="s">
         <v>21</v>
       </c>
       <c r="K299" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="300" spans="1:12" x14ac:dyDescent="0.3">
@@ -5654,16 +5657,16 @@
         <v>617771</v>
       </c>
       <c r="B300" s="5" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C300" s="5" t="s">
         <v>180</v>
       </c>
       <c r="D300" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="E300" s="6" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="301" spans="1:12" x14ac:dyDescent="0.3">
@@ -5671,37 +5674,37 @@
         <v>230325</v>
       </c>
       <c r="B301" s="5" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C301" s="5" t="s">
         <v>180</v>
       </c>
       <c r="D301" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="E301" s="6" t="s">
         <v>17</v>
       </c>
       <c r="F301" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="G301" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H301" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I301" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="J301" t="s">
         <v>21</v>
       </c>
       <c r="K301" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="L301" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
   </sheetData>
@@ -5727,10 +5730,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -5738,7 +5741,7 @@
         <v>869123</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -5746,7 +5749,7 @@
         <v>300076</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -5754,7 +5757,7 @@
         <v>321843</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -5762,7 +5765,7 @@
         <v>650674</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -5770,7 +5773,7 @@
         <v>289205</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -5778,7 +5781,7 @@
         <v>141787</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -5786,7 +5789,7 @@
         <v>287679</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -5794,7 +5797,7 @@
         <v>647487</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -5802,7 +5805,7 @@
         <v>451487</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -5810,7 +5813,7 @@
         <v>861671</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -5818,7 +5821,7 @@
         <v>316094</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -5826,7 +5829,7 @@
         <v>924424</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -5834,7 +5837,7 @@
         <v>918170</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -5842,7 +5845,7 @@
         <v>617771</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -5850,7 +5853,7 @@
         <v>230325</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
   </sheetData>
@@ -5871,10 +5874,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -5882,7 +5885,7 @@
         <v>789271</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -5890,7 +5893,7 @@
         <v>533772</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -5898,7 +5901,7 @@
         <v>979471</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -5906,7 +5909,7 @@
         <v>433534</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -5914,7 +5917,7 @@
         <v>185957</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -5922,7 +5925,7 @@
         <v>997539</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -5930,7 +5933,7 @@
         <v>581651</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -5938,7 +5941,7 @@
         <v>493614</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -5946,7 +5949,7 @@
         <v>869576</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -5954,7 +5957,7 @@
         <v>166937</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -5981,10 +5984,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="I1" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -5998,7 +6001,7 @@
         <v>14</v>
       </c>
       <c r="I2" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -6160,7 +6163,7 @@
         <v>590307</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>180</v>
@@ -6171,7 +6174,7 @@
         <v>847633</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>180</v>
@@ -6182,7 +6185,7 @@
         <v>538067</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>180</v>
@@ -6193,7 +6196,7 @@
         <v>889142</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>180</v>
@@ -6204,7 +6207,7 @@
         <v>988429</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>180</v>
@@ -6215,7 +6218,7 @@
         <v>159320</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>180</v>
@@ -6226,7 +6229,7 @@
         <v>985070</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>180</v>
@@ -6237,7 +6240,7 @@
         <v>872696</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>180</v>
@@ -6248,7 +6251,7 @@
         <v>645107</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>180</v>
@@ -6259,7 +6262,7 @@
         <v>213190</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>180</v>
@@ -6270,7 +6273,7 @@
         <v>170406</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>180</v>
@@ -6281,7 +6284,7 @@
         <v>588655</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>180</v>
@@ -6292,7 +6295,7 @@
         <v>441310</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>180</v>
@@ -6303,7 +6306,7 @@
         <v>312435</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>180</v>
@@ -6314,7 +6317,7 @@
         <v>505418</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>180</v>

</xml_diff>

<commit_message>
add download data buton
</commit_message>
<xml_diff>
--- a/Data/acount and passwords.xlsx
+++ b/Data/acount and passwords.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Oz\fiveer\Dani_Velinchick\KrohnApp\python_codes\COBIMINDEX\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47BC6995-2594-473A-91CB-C80BF83DAB64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED46D95-E966-4D78-A2BE-91846D3B1E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1622,7 +1622,7 @@
   <dimension ref="A1:M301"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
switch levels 3 and 4
</commit_message>
<xml_diff>
--- a/Data/acount and passwords.xlsx
+++ b/Data/acount and passwords.xlsx
@@ -1512,7 +1512,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Hila Askayo</t>
+          <t>General</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1538,6 +1538,11 @@
       <c r="K17" t="inlineStr">
         <is>
           <t>2025-04-01</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>blocked</t>
         </is>
       </c>
     </row>
@@ -5940,6 +5945,11 @@
           <t>02-101</t>
         </is>
       </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>Ganit Goren</t>
+        </is>
+      </c>
       <c r="F179" t="inlineStr">
         <is>
           <t>Hila Askayo</t>
@@ -6087,7 +6097,37 @@
       </c>
       <c r="D182" s="18" t="inlineStr">
         <is>
-          <t>Allocated for E-Patient</t>
+          <t>02-103</t>
+        </is>
+      </c>
+      <c r="F182" t="inlineStr">
+        <is>
+          <t>Hila Askayo</t>
+        </is>
+      </c>
+      <c r="G182" t="inlineStr">
+        <is>
+          <t>2024-06-20</t>
+        </is>
+      </c>
+      <c r="H182" t="inlineStr">
+        <is>
+          <t>2024-09-24</t>
+        </is>
+      </c>
+      <c r="I182" t="inlineStr">
+        <is>
+          <t>2024-12-23</t>
+        </is>
+      </c>
+      <c r="J182" t="inlineStr">
+        <is>
+          <t>2025-03-23</t>
+        </is>
+      </c>
+      <c r="K182" t="inlineStr">
+        <is>
+          <t>2025-06-21</t>
         </is>
       </c>
     </row>
@@ -6107,7 +6147,37 @@
       </c>
       <c r="D183" s="18" t="inlineStr">
         <is>
-          <t>Allocated for E-Patient</t>
+          <t>04-190</t>
+        </is>
+      </c>
+      <c r="F183" t="inlineStr">
+        <is>
+          <t>Hila Askayo</t>
+        </is>
+      </c>
+      <c r="G183" t="inlineStr">
+        <is>
+          <t>2024-06-16</t>
+        </is>
+      </c>
+      <c r="H183" t="inlineStr">
+        <is>
+          <t>2024-09-16</t>
+        </is>
+      </c>
+      <c r="I183" t="inlineStr">
+        <is>
+          <t>2024-12-15</t>
+        </is>
+      </c>
+      <c r="J183" t="inlineStr">
+        <is>
+          <t>2025-03-15</t>
+        </is>
+      </c>
+      <c r="K183" t="inlineStr">
+        <is>
+          <t>2025-06-13</t>
         </is>
       </c>
     </row>
@@ -6127,7 +6197,37 @@
       </c>
       <c r="D184" s="18" t="inlineStr">
         <is>
-          <t>Allocated for E-Patient</t>
+          <t>01-016</t>
+        </is>
+      </c>
+      <c r="F184" t="inlineStr">
+        <is>
+          <t>Hila Askayo</t>
+        </is>
+      </c>
+      <c r="G184" t="inlineStr">
+        <is>
+          <t>2024-06-24</t>
+        </is>
+      </c>
+      <c r="H184" t="inlineStr">
+        <is>
+          <t>2024-09-24</t>
+        </is>
+      </c>
+      <c r="I184" t="inlineStr">
+        <is>
+          <t>2024-12-23</t>
+        </is>
+      </c>
+      <c r="J184" t="inlineStr">
+        <is>
+          <t>2025-03-23</t>
+        </is>
+      </c>
+      <c r="K184" t="inlineStr">
+        <is>
+          <t>2025-06-21</t>
         </is>
       </c>
     </row>

</xml_diff>